<commit_message>
updated template and example for importing samples
</commit_message>
<xml_diff>
--- a/static/scats_upload_example.xlsx
+++ b/static/scats_upload_example.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="104">
   <si>
     <t xml:space="preserve">scat_id</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">wa_code</t>
   </si>
   <si>
-    <t xml:space="preserve">genotype_id</t>
+    <t xml:space="preserve">sample_type</t>
   </si>
   <si>
     <t xml:space="preserve">sampling_type</t>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">E200503APAPJF01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excrement</t>
   </si>
   <si>
     <t xml:space="preserve">Opportunistic</t>
@@ -488,6 +491,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEEEEEC"/>
+          <bgColor rgb="FF2D2D2D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -498,25 +518,25 @@
   </sheetPr>
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.35546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="44.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="44.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="23.3"/>
@@ -602,35 +622,37 @@
         <v>43954</v>
       </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" s="11" t="n">
         <v>484424</v>
@@ -639,50 +661,53 @@
         <v>4933576</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U2" s="8"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>43955</v>
       </c>
+      <c r="D3" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="13"/>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P3" s="14" t="n">
         <v>478158</v>
@@ -691,54 +716,57 @@
         <v>4941509</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D4" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P4" s="14" t="n">
         <v>404266</v>
@@ -747,54 +775,57 @@
         <v>4885098</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P5" s="14" t="n">
         <v>362465</v>
@@ -803,52 +834,55 @@
         <v>4922505</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P6" s="14" t="n">
         <v>394822</v>
@@ -857,52 +891,55 @@
         <v>4885494</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P7" s="14" t="n">
         <v>394735</v>
@@ -911,52 +948,55 @@
         <v>4885259</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P8" s="14" t="n">
         <v>393705</v>
@@ -965,52 +1005,55 @@
         <v>4886299</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D9" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P9" s="14" t="n">
         <v>393700</v>
@@ -1019,52 +1062,55 @@
         <v>4886303</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P10" s="14" t="n">
         <v>393700</v>
@@ -1073,52 +1119,55 @@
         <v>4886303</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P11" s="14" t="n">
         <v>393101</v>
@@ -1127,52 +1176,55 @@
         <v>4887340</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>44105</v>
       </c>
+      <c r="D12" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P12" s="14" t="n">
         <v>393484</v>
@@ -1181,55 +1233,58 @@
         <v>4887697</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U12" s="8"/>
     </row>
-    <row r="13" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>44105</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P13" s="14" t="n">
         <v>398861</v>
@@ -1238,57 +1293,60 @@
         <v>4887335</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>44105</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P14" s="14" t="n">
         <v>398613</v>
@@ -1297,51 +1355,54 @@
         <v>4888051</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>44136</v>
       </c>
+      <c r="D15" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P15" s="14" t="n">
         <v>476406</v>
@@ -1350,52 +1411,55 @@
         <v>4937706</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>44136</v>
       </c>
+      <c r="D16" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P16" s="14" t="n">
         <v>488481</v>
@@ -1404,52 +1468,55 @@
         <v>4960534</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U16" s="8"/>
     </row>
-    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>44136</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P17" s="14" t="n">
         <v>364729</v>
@@ -1458,52 +1525,55 @@
         <v>4903383</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U17" s="8"/>
     </row>
-    <row r="18" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>44136</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P18" s="14" t="n">
         <v>364301</v>
@@ -1512,52 +1582,55 @@
         <v>4903743</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U18" s="8"/>
     </row>
-    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>44136</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P19" s="14" t="n">
         <v>360212</v>
@@ -1566,52 +1639,55 @@
         <v>4895997</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U19" s="8"/>
     </row>
-    <row r="20" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>44136</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P20" s="14" t="n">
         <v>399117</v>
@@ -1620,49 +1696,52 @@
         <v>4889603</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S20" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T20" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>44136</v>
       </c>
+      <c r="D21" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P21" s="14" t="n">
         <v>399828</v>
@@ -1671,49 +1750,52 @@
         <v>4891769</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S21" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>44136</v>
       </c>
+      <c r="D22" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P22" s="14" t="n">
         <v>400503</v>
@@ -1722,49 +1804,52 @@
         <v>4891036</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S22" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T22" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>44136</v>
       </c>
+      <c r="D23" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P23" s="14" t="n">
         <v>400504</v>
@@ -1773,49 +1858,52 @@
         <v>4891036</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S23" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T23" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>44136</v>
       </c>
+      <c r="D24" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E24" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P24" s="14" t="n">
         <v>400503</v>
@@ -1824,49 +1912,52 @@
         <v>4891037</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S24" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T24" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>44136</v>
       </c>
+      <c r="D25" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E25" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P25" s="14" t="n">
         <v>400504</v>
@@ -1875,38 +1966,38 @@
         <v>4891037</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S25" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T25" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U25" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" prompt=" - " showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="L2:N2 L4:N25" type="list">
-      <formula1>#REF!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="K3" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt=" - " showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="L2:N2 L4:N25" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt=" - " showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E2:E4 L3:N3 E5:E25" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="K3" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="K2 K4:K25" type="list">
-      <formula1>#REF!</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt=" - " showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E2:E4 L3:N3 E5:E25" type="list">
+      <formula1>#ref!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="K2 K4:K25" type="list">
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>